<commit_message>
auto: update vanuit Teams
</commit_message>
<xml_diff>
--- a/Coachingslijst.xlsx
+++ b/Coachingslijst.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://delijn.sharepoint.com/teams/CTM-Opmakensteekkaarten-Coachingslijst/Gedeelde documenten/Coachingslijst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5924" documentId="13_ncr:1_{51182797-F005-4DB1-88AE-A2BD37A2289A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E92144E2-0FDF-4608-A3A3-51B33B582A89}"/>
+  <xr:revisionPtr revIDLastSave="5927" documentId="13_ncr:1_{51182797-F005-4DB1-88AE-A2BD37A2289A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A7EFBA3-B0FC-4B6F-A271-51A1DB322973}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-180" windowWidth="29040" windowHeight="15720" tabRatio="456" xr2:uid="{F593FE5F-E761-4E50-85A0-6D382CBE16EB}"/>
   </bookViews>
@@ -4188,8 +4188,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9C435D86-3872-4CC1-9A54-581B1CD3E3B5}" name="Tabel2" displayName="Tabel2" ref="A1:S93" totalsRowShown="0">
-  <autoFilter ref="A1:S93" xr:uid="{9C435D86-3872-4CC1-9A54-581B1CD3E3B5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9C435D86-3872-4CC1-9A54-581B1CD3E3B5}" name="Tabel2" displayName="Tabel2" ref="A1:S91" totalsRowShown="0">
+  <autoFilter ref="A1:S91" xr:uid="{9C435D86-3872-4CC1-9A54-581B1CD3E3B5}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S79">
     <sortCondition ref="B1:B79"/>
   </sortState>
@@ -4603,10 +4603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310BB95E-2952-4B45-98D4-2E7AF749FAF9}">
-  <dimension ref="A1:S93"/>
+  <dimension ref="A1:S91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K84" sqref="K84"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89:XFD90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7661,6 +7661,12 @@
         <f>VLOOKUP(Tabel2[[#This Row],[P-nr]],'data Chauffeur'!A:F,5,FALSE)</f>
         <v>BO15</v>
       </c>
+      <c r="K84" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L84" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="85" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E85" t="e">
@@ -7833,56 +7839,6 @@
         <v>#N/A</v>
       </c>
       <c r="J91" t="e">
-        <f>VLOOKUP(Tabel2[[#This Row],[P-nr]],'data Chauffeur'!A:F,5,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="92" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="E92" t="e">
-        <f>VLOOKUP(Tabel2[[#This Row],[P-nr]],'data Chauffeur'!A:F,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F92" t="e">
-        <f>VLOOKUP(Tabel2[[#This Row],[P-nr]],'data Chauffeur'!A:F,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G92" t="e">
-        <f>_xlfn.CONCAT(Tabel2[[#This Row],[P-nr]]," ",Tabel2[[#This Row],[Naam]]," ",Tabel2[[#This Row],[Voornaam]]," ",)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H92" t="s">
-        <v>32</v>
-      </c>
-      <c r="I92" t="e">
-        <f>VLOOKUP(Tabel2[[#This Row],[P-nr]],'data Chauffeur'!A:F,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J92" t="e">
-        <f>VLOOKUP(Tabel2[[#This Row],[P-nr]],'data Chauffeur'!A:F,5,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="93" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="E93" t="e">
-        <f>VLOOKUP(Tabel2[[#This Row],[P-nr]],'data Chauffeur'!A:F,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F93" t="e">
-        <f>VLOOKUP(Tabel2[[#This Row],[P-nr]],'data Chauffeur'!A:F,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G93" t="e">
-        <f>_xlfn.CONCAT(Tabel2[[#This Row],[P-nr]]," ",Tabel2[[#This Row],[Naam]]," ",Tabel2[[#This Row],[Voornaam]]," ",)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H93" t="s">
-        <v>32</v>
-      </c>
-      <c r="I93" t="e">
-        <f>VLOOKUP(Tabel2[[#This Row],[P-nr]],'data Chauffeur'!A:F,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J93" t="e">
         <f>VLOOKUP(Tabel2[[#This Row],[P-nr]],'data Chauffeur'!A:F,5,FALSE)</f>
         <v>#N/A</v>
       </c>
@@ -16305,7 +16261,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <f>COUNTIF(Coaching!I1:I9986,Tabel1[[#This Row],[Teamcoach]])</f>
+        <f>COUNTIF(Coaching!I1:I9984,Tabel1[[#This Row],[Teamcoach]])</f>
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -16322,7 +16278,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <f>COUNTIF(Coaching!I2:I9987,Tabel1[[#This Row],[Teamcoach]])</f>
+        <f>COUNTIF(Coaching!I2:I9985,Tabel1[[#This Row],[Teamcoach]])</f>
         <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -16339,7 +16295,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <f>COUNTIF(Coaching!I2:I9988,Tabel1[[#This Row],[Teamcoach]])</f>
+        <f>COUNTIF(Coaching!I2:I9986,Tabel1[[#This Row],[Teamcoach]])</f>
         <v>13</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -16356,7 +16312,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <f>COUNTIF(Coaching!I3:I9989,Tabel1[[#This Row],[Teamcoach]])</f>
+        <f>COUNTIF(Coaching!I3:I9987,Tabel1[[#This Row],[Teamcoach]])</f>
         <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -16373,7 +16329,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <f>COUNTIF(Coaching!I4:I9990,Tabel1[[#This Row],[Teamcoach]])</f>
+        <f>COUNTIF(Coaching!I4:I9988,Tabel1[[#This Row],[Teamcoach]])</f>
         <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -16390,7 +16346,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <f>COUNTIF(Coaching!I5:I9991,Tabel1[[#This Row],[Teamcoach]])</f>
+        <f>COUNTIF(Coaching!I5:I9989,Tabel1[[#This Row],[Teamcoach]])</f>
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -16407,7 +16363,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <f>COUNTIF(Coaching!I6:I9992,Tabel1[[#This Row],[Teamcoach]])</f>
+        <f>COUNTIF(Coaching!I6:I9990,Tabel1[[#This Row],[Teamcoach]])</f>
         <v>11</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -16424,7 +16380,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <f>COUNTIF(Coaching!I6:I9993,Tabel1[[#This Row],[Teamcoach]])</f>
+        <f>COUNTIF(Coaching!I6:I9991,Tabel1[[#This Row],[Teamcoach]])</f>
         <v>10</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -28454,21 +28410,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BABA40AC322E4247AE7CB802C219210E" ma:contentTypeVersion="4" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="091f22780d69c37ad0a887b10b1a0799">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d2bfb4ca-6bc6-4c14-a954-a38929ece6e4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="006df783f42031eefccbb2b77ef17bef" ns2:_="">
     <xsd:import namespace="d2bfb4ca-6bc6-4c14-a954-a38929ece6e4"/>
@@ -28612,24 +28553,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6B7A3F1-CC45-4FC0-B485-69FB7DFFE38E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AABF25EA-A7EB-41E2-8065-BEF79D9BAEF4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A25AB59E-5CCD-4E14-BFB6-F23F69C5C3AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -28645,4 +28584,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AABF25EA-A7EB-41E2-8065-BEF79D9BAEF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6B7A3F1-CC45-4FC0-B485-69FB7DFFE38E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>